<commit_message>
Se revisa la ortografia del plan de pruebas
</commit_message>
<xml_diff>
--- a/Plan-de-Calidad-Mobile.xlsx
+++ b/Plan-de-Calidad-Mobile.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DISENO11\IdeaProjects\sofka\C1-2023-QA-Auto-Taller-Mobile\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6B7C2F1-3AD7-4662-983D-93ADB14A3F02}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{412507C8-8D8D-4757-ADD4-BCE603D25551}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1111,7 +1111,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J1" sqref="J1:J1048576"/>
+      <selection pane="bottomLeft" activeCell="G2" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>